<commit_message>
## [2026-02-12] 準備處理 Dexie
</commit_message>
<xml_diff>
--- a/sheets/2026NonBlockingLife.xlsx
+++ b/sheets/2026NonBlockingLife.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d39fb11249e9e67/Documents/2026/NonBlockingLife/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_63D8BEEEA8F590E3939130FE62F4A9A5849807A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26DFAF07-FAD5-46D5-8FF6-6A5582BB4CE8}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_63D8BEEEA8F590E3939130FE62F4A9A5849807A9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6588497B-6F24-45C6-9B37-CBB7C1652E3B}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="2550" windowWidth="10500" windowHeight="10500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>Timestamp</t>
   </si>
@@ -212,7 +212,7 @@
     <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="179" formatCode="yyyy/m/d\ am/pm\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -238,6 +238,13 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -259,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -268,6 +275,7 @@
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -314,6 +322,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1989,16 +2001,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2007,6 +2019,9 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>